<commit_message>
added Frankreich data change
</commit_message>
<xml_diff>
--- a/data/Mapping the Atlas.xlsx
+++ b/data/Mapping the Atlas.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelilletschko/Documents/Akademisches/Germanistik/Christoph Ransmayr/0_Mapping Ransmayr/1_Band/Einleitung/Marcel-Teil/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\m.illetschko\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F24C889A-E27E-1243-B100-C4B9F5BEFD12}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{63574BCD-3B72-47D8-9B30-59218728FA5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="43900" windowHeight="26740" xr2:uid="{33803157-FF31-BB4F-88D2-C1B07BDFCD58}"/>
+    <workbookView xWindow="-28920" yWindow="1095" windowWidth="29040" windowHeight="15840" xr2:uid="{33803157-FF31-BB4F-88D2-C1B07BDFCD58}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -26,11 +26,11 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="10" r:id="rId8"/>
-    <pivotCache cacheId="11" r:id="rId9"/>
-    <pivotCache cacheId="12" r:id="rId10"/>
-    <pivotCache cacheId="13" r:id="rId11"/>
-    <pivotCache cacheId="14" r:id="rId12"/>
+    <pivotCache cacheId="0" r:id="rId8"/>
+    <pivotCache cacheId="1" r:id="rId9"/>
+    <pivotCache cacheId="2" r:id="rId10"/>
+    <pivotCache cacheId="3" r:id="rId11"/>
+    <pivotCache cacheId="4" r:id="rId12"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -6204,21 +6204,6 @@
     <t>14.12457</t>
   </si>
   <si>
-    <t>2.5333332</t>
-  </si>
-  <si>
-    <t>2.5333333</t>
-  </si>
-  <si>
-    <t>2.5333334</t>
-  </si>
-  <si>
-    <t>2.5333335</t>
-  </si>
-  <si>
-    <t>2.5333336</t>
-  </si>
-  <si>
     <t>35.943752</t>
   </si>
   <si>
@@ -6574,15 +6559,37 @@
   </si>
   <si>
     <t>87.093</t>
+  </si>
+  <si>
+    <t>2.5333</t>
+  </si>
+  <si>
+    <t>2.53334</t>
+  </si>
+  <si>
+    <t>2.53336</t>
+  </si>
+  <si>
+    <t>2.53338</t>
+  </si>
+  <si>
+    <t>2.53340</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10">
+  <fonts count="11">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -6667,32 +6674,32 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="2" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -6701,7 +6708,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Link" xfId="1" builtinId="8"/>
@@ -22557,7 +22565,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF0B8061-5D4D-F04A-ACE0-B39B2B8B537A}" name="PivotTable3" cacheId="10" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{EF0B8061-5D4D-F04A-ACE0-B39B2B8B537A}" name="PivotTable3" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B624" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -25073,7 +25081,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5F40172-D960-3A44-8977-FC1DC6A5E078}" name="PivotTable4" cacheId="11" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{D5F40172-D960-3A44-8977-FC1DC6A5E078}" name="PivotTable4" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B108" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -25525,7 +25533,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4C13BCF-B99F-9F4F-90C3-E819DB696FC3}" name="PivotTable5" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{A4C13BCF-B99F-9F4F-90C3-E819DB696FC3}" name="PivotTable5" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B24" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -25641,7 +25649,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7965CEC4-E306-A842-B3FA-5C1232DBCC36}" name="PivotTable6" cacheId="13" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{7965CEC4-E306-A842-B3FA-5C1232DBCC36}" name="PivotTable6" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:C146" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -26262,7 +26270,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4BFB8E4-9F46-354E-8A79-706F7DAAE24C}" name="PivotTable8" cacheId="14" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{B4BFB8E4-9F46-354E-8A79-706F7DAAE24C}" name="PivotTable8" cacheId="4" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Werte" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:B82" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="1">
     <pivotField axis="axisRow" dataField="1" showAll="0">
@@ -26909,19 +26917,19 @@
   <dimension ref="A1:K819"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D828" sqref="D828"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="30.83203125" style="4" customWidth="1"/>
-    <col min="4" max="7" width="24.83203125" style="4" customWidth="1"/>
-    <col min="8" max="8" width="24.83203125" style="8" customWidth="1"/>
-    <col min="9" max="9" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.83203125" style="4" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="2" width="10.875" style="4"/>
+    <col min="3" max="3" width="30.875" style="4" customWidth="1"/>
+    <col min="4" max="7" width="24.875" style="4" customWidth="1"/>
+    <col min="8" max="8" width="24.875" style="8" customWidth="1"/>
+    <col min="9" max="9" width="11.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="24.875" style="4" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="1"/>
+    <col min="12" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15">
@@ -27016,7 +27024,7 @@
         <v>1341</v>
       </c>
       <c r="I3" s="10" t="s">
-        <v>2155</v>
+        <v>2150</v>
       </c>
       <c r="J3" s="4">
         <v>1</v>
@@ -27346,7 +27354,7 @@
         <v>714</v>
       </c>
       <c r="I13" s="10" t="s">
-        <v>2123</v>
+        <v>2118</v>
       </c>
       <c r="J13" s="4">
         <v>1</v>
@@ -27379,7 +27387,7 @@
         <v>716</v>
       </c>
       <c r="I14" s="10" t="s">
-        <v>2137</v>
+        <v>2132</v>
       </c>
       <c r="J14" s="4">
         <v>1</v>
@@ -27511,7 +27519,7 @@
         <v>724</v>
       </c>
       <c r="I18" s="10" t="s">
-        <v>2138</v>
+        <v>2133</v>
       </c>
       <c r="J18" s="4">
         <v>1</v>
@@ -27610,7 +27618,7 @@
         <v>1345</v>
       </c>
       <c r="I21" s="10" t="s">
-        <v>2134</v>
+        <v>2129</v>
       </c>
       <c r="J21" s="4">
         <v>1</v>
@@ -27643,7 +27651,7 @@
         <v>714</v>
       </c>
       <c r="I22" s="10" t="s">
-        <v>2124</v>
+        <v>2119</v>
       </c>
       <c r="J22" s="4">
         <v>1</v>
@@ -27676,7 +27684,7 @@
         <v>1346</v>
       </c>
       <c r="I23" s="10" t="s">
-        <v>2142</v>
+        <v>2137</v>
       </c>
       <c r="J23" s="4">
         <v>1</v>
@@ -27709,7 +27717,7 @@
         <v>724</v>
       </c>
       <c r="I24" s="10" t="s">
-        <v>2139</v>
+        <v>2134</v>
       </c>
       <c r="J24" s="4">
         <v>1</v>
@@ -27874,7 +27882,7 @@
         <v>1350</v>
       </c>
       <c r="I29" s="10" t="s">
-        <v>2147</v>
+        <v>2142</v>
       </c>
       <c r="J29" s="4">
         <v>1</v>
@@ -28104,8 +28112,8 @@
       <c r="H36" s="13" t="s">
         <v>1357</v>
       </c>
-      <c r="I36" s="10" t="s">
-        <v>2051</v>
+      <c r="I36" s="26" t="s">
+        <v>2170</v>
       </c>
       <c r="J36" s="4">
         <v>1</v>
@@ -28138,7 +28146,7 @@
         <v>1350</v>
       </c>
       <c r="I37" s="10" t="s">
-        <v>2148</v>
+        <v>2143</v>
       </c>
       <c r="J37" s="4">
         <v>1</v>
@@ -28171,7 +28179,7 @@
         <v>1358</v>
       </c>
       <c r="I38" s="10" t="s">
-        <v>2086</v>
+        <v>2081</v>
       </c>
       <c r="J38" s="18">
         <v>0</v>
@@ -29491,7 +29499,7 @@
         <v>1387</v>
       </c>
       <c r="I78" s="10" t="s">
-        <v>2079</v>
+        <v>2074</v>
       </c>
       <c r="J78" s="4">
         <v>1</v>
@@ -29656,7 +29664,7 @@
         <v>1397</v>
       </c>
       <c r="I83" s="10" t="s">
-        <v>2074</v>
+        <v>2069</v>
       </c>
       <c r="J83" s="4">
         <v>1</v>
@@ -29689,7 +29697,7 @@
         <v>1398</v>
       </c>
       <c r="I84" s="10" t="s">
-        <v>2077</v>
+        <v>2072</v>
       </c>
       <c r="J84" s="4">
         <v>1</v>
@@ -29854,7 +29862,7 @@
         <v>1402</v>
       </c>
       <c r="I89" s="10" t="s">
-        <v>2144</v>
+        <v>2139</v>
       </c>
       <c r="J89" s="4">
         <v>1</v>
@@ -29920,7 +29928,7 @@
         <v>1404</v>
       </c>
       <c r="I91" s="10" t="s">
-        <v>2143</v>
+        <v>2138</v>
       </c>
       <c r="J91" s="4">
         <v>1</v>
@@ -30382,7 +30390,7 @@
         <v>1358</v>
       </c>
       <c r="I105" s="10" t="s">
-        <v>2087</v>
+        <v>2082</v>
       </c>
       <c r="J105" s="18">
         <v>0</v>
@@ -30481,7 +30489,7 @@
         <v>1416</v>
       </c>
       <c r="I108" s="10" t="s">
-        <v>2109</v>
+        <v>2104</v>
       </c>
       <c r="J108" s="4">
         <v>1</v>
@@ -30745,7 +30753,7 @@
         <v>1421</v>
       </c>
       <c r="I116" s="10" t="s">
-        <v>2108</v>
+        <v>2103</v>
       </c>
       <c r="J116" s="4">
         <v>1</v>
@@ -30811,7 +30819,7 @@
         <v>1423</v>
       </c>
       <c r="I118" s="10" t="s">
-        <v>2117</v>
+        <v>2112</v>
       </c>
       <c r="J118" s="4">
         <v>1</v>
@@ -30877,7 +30885,7 @@
         <v>1423</v>
       </c>
       <c r="I120" s="10" t="s">
-        <v>2119</v>
+        <v>2114</v>
       </c>
       <c r="J120" s="4">
         <v>1</v>
@@ -30910,7 +30918,7 @@
         <v>1425</v>
       </c>
       <c r="I121" s="10" t="s">
-        <v>2120</v>
+        <v>2115</v>
       </c>
       <c r="J121" s="4">
         <v>1</v>
@@ -30976,7 +30984,7 @@
         <v>1416</v>
       </c>
       <c r="I123" s="10" t="s">
-        <v>2110</v>
+        <v>2105</v>
       </c>
       <c r="J123" s="4">
         <v>1</v>
@@ -31702,7 +31710,7 @@
         <v>1350</v>
       </c>
       <c r="I145" s="10" t="s">
-        <v>2149</v>
+        <v>2144</v>
       </c>
       <c r="J145" s="4">
         <v>1</v>
@@ -31933,7 +31941,7 @@
         <v>1449</v>
       </c>
       <c r="I152" s="10" t="s">
-        <v>2072</v>
+        <v>2067</v>
       </c>
       <c r="J152" s="4">
         <v>1</v>
@@ -32098,7 +32106,7 @@
         <v>1453</v>
       </c>
       <c r="I157" s="10" t="s">
-        <v>2097</v>
+        <v>2092</v>
       </c>
       <c r="J157" s="18">
         <v>0</v>
@@ -32131,7 +32139,7 @@
         <v>1387</v>
       </c>
       <c r="I158" s="10" t="s">
-        <v>2080</v>
+        <v>2075</v>
       </c>
       <c r="J158" s="4">
         <v>1</v>
@@ -32230,7 +32238,7 @@
         <v>1456</v>
       </c>
       <c r="I161" s="10" t="s">
-        <v>2088</v>
+        <v>2083</v>
       </c>
       <c r="J161" s="4">
         <v>1</v>
@@ -32263,7 +32271,7 @@
         <v>1387</v>
       </c>
       <c r="I162" s="10" t="s">
-        <v>2081</v>
+        <v>2076</v>
       </c>
       <c r="J162" s="4">
         <v>1</v>
@@ -33616,7 +33624,7 @@
         <v>1367</v>
       </c>
       <c r="I203" s="10" t="s">
-        <v>2153</v>
+        <v>2148</v>
       </c>
       <c r="J203" s="18">
         <v>0</v>
@@ -33814,7 +33822,7 @@
         <v>1341</v>
       </c>
       <c r="I209" s="10" t="s">
-        <v>2156</v>
+        <v>2151</v>
       </c>
       <c r="J209" s="4">
         <v>1</v>
@@ -33847,7 +33855,7 @@
         <v>1493</v>
       </c>
       <c r="I210" s="10" t="s">
-        <v>2058</v>
+        <v>2053</v>
       </c>
       <c r="J210" s="4">
         <v>1</v>
@@ -34573,7 +34581,7 @@
         <v>1495</v>
       </c>
       <c r="I232" s="10" t="s">
-        <v>2163</v>
+        <v>2158</v>
       </c>
       <c r="J232" s="19">
         <v>0</v>
@@ -34738,7 +34746,7 @@
         <v>1350</v>
       </c>
       <c r="I237" s="10" t="s">
-        <v>2150</v>
+        <v>2145</v>
       </c>
       <c r="J237" s="4">
         <v>1</v>
@@ -34771,7 +34779,7 @@
         <v>1350</v>
       </c>
       <c r="I238" s="10" t="s">
-        <v>2151</v>
+        <v>2146</v>
       </c>
       <c r="J238" s="4">
         <v>1</v>
@@ -34903,7 +34911,7 @@
         <v>1493</v>
       </c>
       <c r="I242" s="10" t="s">
-        <v>2059</v>
+        <v>2054</v>
       </c>
       <c r="J242" s="4">
         <v>1</v>
@@ -35035,7 +35043,7 @@
         <v>1358</v>
       </c>
       <c r="I246" s="10" t="s">
-        <v>2089</v>
+        <v>2084</v>
       </c>
       <c r="J246" s="18">
         <v>0</v>
@@ -35068,7 +35076,7 @@
         <v>1863</v>
       </c>
       <c r="I247" s="10" t="s">
-        <v>2122</v>
+        <v>2117</v>
       </c>
       <c r="J247" s="4">
         <v>1</v>
@@ -35167,7 +35175,7 @@
         <v>1678</v>
       </c>
       <c r="I250" s="10" t="s">
-        <v>2121</v>
+        <v>2116</v>
       </c>
       <c r="J250" s="4">
         <v>1</v>
@@ -35332,7 +35340,7 @@
         <v>1828</v>
       </c>
       <c r="I255" s="10" t="s">
-        <v>2132</v>
+        <v>2127</v>
       </c>
       <c r="J255" s="4">
         <v>1</v>
@@ -35529,8 +35537,8 @@
       <c r="H261" s="13" t="s">
         <v>1357</v>
       </c>
-      <c r="I261" s="10" t="s">
-        <v>2052</v>
+      <c r="I261" s="26" t="s">
+        <v>2171</v>
       </c>
       <c r="J261" s="4">
         <v>1</v>
@@ -35629,7 +35637,7 @@
         <v>1493</v>
       </c>
       <c r="I264" s="10" t="s">
-        <v>2060</v>
+        <v>2055</v>
       </c>
       <c r="J264" s="4">
         <v>1</v>
@@ -36157,7 +36165,7 @@
         <v>1402</v>
       </c>
       <c r="I280" s="10" t="s">
-        <v>2145</v>
+        <v>2140</v>
       </c>
       <c r="J280" s="4">
         <v>1</v>
@@ -36454,7 +36462,7 @@
         <v>1402</v>
       </c>
       <c r="I289" s="10" t="s">
-        <v>2146</v>
+        <v>2141</v>
       </c>
       <c r="J289" s="4">
         <v>1</v>
@@ -36553,7 +36561,7 @@
         <v>1624</v>
       </c>
       <c r="I292" s="10" t="s">
-        <v>2103</v>
+        <v>2098</v>
       </c>
       <c r="J292" s="4">
         <v>1</v>
@@ -36619,7 +36627,7 @@
         <v>1625</v>
       </c>
       <c r="I294" s="10" t="s">
-        <v>2096</v>
+        <v>2091</v>
       </c>
       <c r="J294" s="4">
         <v>1</v>
@@ -36685,7 +36693,7 @@
         <v>1751</v>
       </c>
       <c r="I296" s="10" t="s">
-        <v>2095</v>
+        <v>2090</v>
       </c>
       <c r="J296" s="4">
         <v>1</v>
@@ -37048,7 +37056,7 @@
         <v>1493</v>
       </c>
       <c r="I307" s="10" t="s">
-        <v>2061</v>
+        <v>2056</v>
       </c>
       <c r="J307" s="4">
         <v>1</v>
@@ -37081,7 +37089,7 @@
         <v>1358</v>
       </c>
       <c r="I308" s="10" t="s">
-        <v>2090</v>
+        <v>2085</v>
       </c>
       <c r="J308" s="18">
         <v>0</v>
@@ -37113,8 +37121,8 @@
       <c r="H309" s="13" t="s">
         <v>1357</v>
       </c>
-      <c r="I309" s="10" t="s">
-        <v>2053</v>
+      <c r="I309" s="26" t="s">
+        <v>2172</v>
       </c>
       <c r="J309" s="4">
         <v>1</v>
@@ -37378,7 +37386,7 @@
         <v>1828</v>
       </c>
       <c r="I317" s="10" t="s">
-        <v>2133</v>
+        <v>2128</v>
       </c>
       <c r="J317" s="4">
         <v>1</v>
@@ -37675,7 +37683,7 @@
         <v>714</v>
       </c>
       <c r="I326" s="10" t="s">
-        <v>2125</v>
+        <v>2120</v>
       </c>
       <c r="J326" s="4">
         <v>1</v>
@@ -37906,7 +37914,7 @@
         <v>1815</v>
       </c>
       <c r="I333" s="10" t="s">
-        <v>2073</v>
+        <v>2068</v>
       </c>
       <c r="J333" s="4">
         <v>1</v>
@@ -38137,7 +38145,7 @@
         <v>1493</v>
       </c>
       <c r="I340" s="10" t="s">
-        <v>2062</v>
+        <v>2057</v>
       </c>
       <c r="J340" s="4">
         <v>1</v>
@@ -38170,7 +38178,7 @@
         <v>1572</v>
       </c>
       <c r="I341" s="10" t="s">
-        <v>2098</v>
+        <v>2093</v>
       </c>
       <c r="J341" s="4">
         <v>1</v>
@@ -38335,7 +38343,7 @@
         <v>1572</v>
       </c>
       <c r="I346" s="10" t="s">
-        <v>2099</v>
+        <v>2094</v>
       </c>
       <c r="J346" s="4">
         <v>1</v>
@@ -38434,7 +38442,7 @@
         <v>1387</v>
       </c>
       <c r="I349" s="10" t="s">
-        <v>2082</v>
+        <v>2077</v>
       </c>
       <c r="J349" s="4">
         <v>1</v>
@@ -38665,7 +38673,7 @@
         <v>1387</v>
       </c>
       <c r="I356" s="10" t="s">
-        <v>2083</v>
+        <v>2078</v>
       </c>
       <c r="J356" s="4">
         <v>1</v>
@@ -38764,7 +38772,7 @@
         <v>1593</v>
       </c>
       <c r="I359" s="10" t="s">
-        <v>2069</v>
+        <v>2064</v>
       </c>
       <c r="J359" s="4">
         <v>1</v>
@@ -38830,7 +38838,7 @@
         <v>1493</v>
       </c>
       <c r="I361" s="10" t="s">
-        <v>2063</v>
+        <v>2058</v>
       </c>
       <c r="J361" s="4">
         <v>1</v>
@@ -38862,8 +38870,8 @@
       <c r="H362" s="13" t="s">
         <v>1357</v>
       </c>
-      <c r="I362" s="10" t="s">
-        <v>2054</v>
+      <c r="I362" s="26" t="s">
+        <v>2173</v>
       </c>
       <c r="J362" s="4">
         <v>1</v>
@@ -38929,7 +38937,7 @@
         <v>1416</v>
       </c>
       <c r="I364" s="10" t="s">
-        <v>2111</v>
+        <v>2106</v>
       </c>
       <c r="J364" s="4">
         <v>1</v>
@@ -38995,7 +39003,7 @@
         <v>1416</v>
       </c>
       <c r="I366" s="10" t="s">
-        <v>2112</v>
+        <v>2107</v>
       </c>
       <c r="J366" s="4">
         <v>1</v>
@@ -39127,7 +39135,7 @@
         <v>1798</v>
       </c>
       <c r="I370" s="10" t="s">
-        <v>2116</v>
+        <v>2111</v>
       </c>
       <c r="J370" s="4">
         <v>1</v>
@@ -39226,7 +39234,7 @@
         <v>1795</v>
       </c>
       <c r="I373" s="10" t="s">
-        <v>2168</v>
+        <v>2163</v>
       </c>
       <c r="J373" s="4">
         <v>1</v>
@@ -39358,7 +39366,7 @@
         <v>1341</v>
       </c>
       <c r="I377" s="10" t="s">
-        <v>2157</v>
+        <v>2152</v>
       </c>
       <c r="J377" s="4">
         <v>1</v>
@@ -39391,7 +39399,7 @@
         <v>1341</v>
       </c>
       <c r="I378" s="10" t="s">
-        <v>2158</v>
+        <v>2153</v>
       </c>
       <c r="J378" s="4">
         <v>1</v>
@@ -39556,7 +39564,7 @@
         <v>1791</v>
       </c>
       <c r="I383" s="10" t="s">
-        <v>2162</v>
+        <v>2157</v>
       </c>
       <c r="J383" s="4">
         <v>1</v>
@@ -39985,7 +39993,7 @@
         <v>1367</v>
       </c>
       <c r="I396" s="10" t="s">
-        <v>2154</v>
+        <v>2149</v>
       </c>
       <c r="J396" s="18">
         <v>0</v>
@@ -40051,7 +40059,7 @@
         <v>1341</v>
       </c>
       <c r="I398" s="10" t="s">
-        <v>2159</v>
+        <v>2154</v>
       </c>
       <c r="J398" s="4">
         <v>1</v>
@@ -40612,7 +40620,7 @@
         <v>1358</v>
       </c>
       <c r="I415" s="10" t="s">
-        <v>2091</v>
+        <v>2086</v>
       </c>
       <c r="J415" s="18">
         <v>0</v>
@@ -41140,7 +41148,7 @@
         <v>1416</v>
       </c>
       <c r="I431" s="10" t="s">
-        <v>2113</v>
+        <v>2108</v>
       </c>
       <c r="J431" s="4">
         <v>1</v>
@@ -41206,7 +41214,7 @@
         <v>1766</v>
       </c>
       <c r="I433" s="10" t="s">
-        <v>2170</v>
+        <v>2165</v>
       </c>
       <c r="J433" s="4">
         <v>1</v>
@@ -41503,7 +41511,7 @@
         <v>1624</v>
       </c>
       <c r="I442" s="10" t="s">
-        <v>2104</v>
+        <v>2099</v>
       </c>
       <c r="J442" s="4">
         <v>1</v>
@@ -41569,7 +41577,7 @@
         <v>1622</v>
       </c>
       <c r="I444" s="10" t="s">
-        <v>2100</v>
+        <v>2095</v>
       </c>
       <c r="J444" s="4">
         <v>1</v>
@@ -41899,7 +41907,7 @@
         <v>1493</v>
       </c>
       <c r="I454" s="10" t="s">
-        <v>2064</v>
+        <v>2059</v>
       </c>
       <c r="J454" s="4">
         <v>1</v>
@@ -42031,7 +42039,7 @@
         <v>1493</v>
       </c>
       <c r="I458" s="10" t="s">
-        <v>2065</v>
+        <v>2060</v>
       </c>
       <c r="J458" s="4">
         <v>1</v>
@@ -42130,7 +42138,7 @@
         <v>1387</v>
       </c>
       <c r="I461" s="10" t="s">
-        <v>2084</v>
+        <v>2079</v>
       </c>
       <c r="J461" s="4">
         <v>1</v>
@@ -42328,7 +42336,7 @@
         <v>1743</v>
       </c>
       <c r="I467" s="10" t="s">
-        <v>2102</v>
+        <v>2097</v>
       </c>
       <c r="J467" s="4">
         <v>1</v>
@@ -42493,7 +42501,7 @@
         <v>1426</v>
       </c>
       <c r="I472" s="10" t="s">
-        <v>2172</v>
+        <v>2167</v>
       </c>
       <c r="J472" s="4">
         <v>1</v>
@@ -42757,7 +42765,7 @@
         <v>1593</v>
       </c>
       <c r="I480" s="10" t="s">
-        <v>2070</v>
+        <v>2065</v>
       </c>
       <c r="J480" s="4">
         <v>1</v>
@@ -42790,7 +42798,7 @@
         <v>1592</v>
       </c>
       <c r="I481" s="10" t="s">
-        <v>2071</v>
+        <v>2066</v>
       </c>
       <c r="J481" s="4">
         <v>1</v>
@@ -43054,7 +43062,7 @@
         <v>1732</v>
       </c>
       <c r="I489" s="10" t="s">
-        <v>2169</v>
+        <v>2164</v>
       </c>
       <c r="J489" s="4">
         <v>1</v>
@@ -43186,7 +43194,7 @@
         <v>1624</v>
       </c>
       <c r="I493" s="10" t="s">
-        <v>2105</v>
+        <v>2100</v>
       </c>
       <c r="J493" s="4">
         <v>1</v>
@@ -43615,7 +43623,7 @@
         <v>1639</v>
       </c>
       <c r="I506" s="10" t="s">
-        <v>2075</v>
+        <v>2070</v>
       </c>
       <c r="J506" s="4">
         <v>1</v>
@@ -43978,7 +43986,7 @@
         <v>1717</v>
       </c>
       <c r="I517" s="10" t="s">
-        <v>2078</v>
+        <v>2073</v>
       </c>
       <c r="J517" s="4">
         <v>1</v>
@@ -44077,7 +44085,7 @@
         <v>1707</v>
       </c>
       <c r="I520" s="10" t="s">
-        <v>2101</v>
+        <v>2096</v>
       </c>
       <c r="J520" s="4">
         <v>1</v>
@@ -44209,7 +44217,7 @@
         <v>1639</v>
       </c>
       <c r="I524" s="10" t="s">
-        <v>2076</v>
+        <v>2071</v>
       </c>
       <c r="J524" s="4">
         <v>1</v>
@@ -44704,7 +44712,7 @@
         <v>714</v>
       </c>
       <c r="I539" s="10" t="s">
-        <v>2126</v>
+        <v>2121</v>
       </c>
       <c r="J539" s="4">
         <v>1</v>
@@ -44737,7 +44745,7 @@
         <v>1576</v>
       </c>
       <c r="I540" s="10" t="s">
-        <v>2131</v>
+        <v>2126</v>
       </c>
       <c r="J540" s="4">
         <v>1</v>
@@ -44770,7 +44778,7 @@
         <v>1701</v>
       </c>
       <c r="I541" s="10" t="s">
-        <v>2165</v>
+        <v>2160</v>
       </c>
       <c r="J541" s="4">
         <v>1</v>
@@ -45694,7 +45702,7 @@
         <v>1423</v>
       </c>
       <c r="I569" s="10" t="s">
-        <v>2118</v>
+        <v>2113</v>
       </c>
       <c r="J569" s="4">
         <v>1</v>
@@ -45958,7 +45966,7 @@
         <v>1677</v>
       </c>
       <c r="I577" s="10" t="s">
-        <v>2167</v>
+        <v>2162</v>
       </c>
       <c r="J577" s="4">
         <v>1</v>
@@ -46024,7 +46032,7 @@
         <v>1624</v>
       </c>
       <c r="I579" s="10" t="s">
-        <v>2106</v>
+        <v>2101</v>
       </c>
       <c r="J579" s="4">
         <v>1</v>
@@ -46156,7 +46164,7 @@
         <v>1670</v>
       </c>
       <c r="I583" s="10" t="s">
-        <v>2085</v>
+        <v>2080</v>
       </c>
       <c r="J583" s="4">
         <v>1</v>
@@ -46486,7 +46494,7 @@
         <v>1341</v>
       </c>
       <c r="I593" s="10" t="s">
-        <v>2160</v>
+        <v>2155</v>
       </c>
       <c r="J593" s="4">
         <v>1</v>
@@ -46519,7 +46527,7 @@
         <v>1341</v>
       </c>
       <c r="I594" s="10" t="s">
-        <v>2161</v>
+        <v>2156</v>
       </c>
       <c r="J594" s="4">
         <v>1</v>
@@ -46651,7 +46659,7 @@
         <v>714</v>
       </c>
       <c r="I598" s="10" t="s">
-        <v>2127</v>
+        <v>2122</v>
       </c>
       <c r="J598" s="4">
         <v>1</v>
@@ -46717,7 +46725,7 @@
         <v>1579</v>
       </c>
       <c r="I600" s="10" t="s">
-        <v>2140</v>
+        <v>2135</v>
       </c>
       <c r="J600" s="4">
         <v>1</v>
@@ -47575,7 +47583,7 @@
         <v>1416</v>
       </c>
       <c r="I626" s="10" t="s">
-        <v>2114</v>
+        <v>2109</v>
       </c>
       <c r="J626" s="4">
         <v>1</v>
@@ -47674,7 +47682,7 @@
         <v>1643</v>
       </c>
       <c r="I629" s="10" t="s">
-        <v>2171</v>
+        <v>2166</v>
       </c>
       <c r="J629" s="4">
         <v>1</v>
@@ -47971,7 +47979,7 @@
         <v>1487</v>
       </c>
       <c r="I638" s="10" t="s">
-        <v>2068</v>
+        <v>2063</v>
       </c>
       <c r="J638" s="4">
         <v>1</v>
@@ -48334,7 +48342,7 @@
         <v>1623</v>
       </c>
       <c r="I649" s="10" t="s">
-        <v>2056</v>
+        <v>2051</v>
       </c>
       <c r="J649" s="4">
         <v>1</v>
@@ -48466,7 +48474,7 @@
         <v>1624</v>
       </c>
       <c r="I653" s="10" t="s">
-        <v>2107</v>
+        <v>2102</v>
       </c>
       <c r="J653" s="4">
         <v>1</v>
@@ -48499,7 +48507,7 @@
         <v>1623</v>
       </c>
       <c r="I654" s="10" t="s">
-        <v>2057</v>
+        <v>2052</v>
       </c>
       <c r="J654" s="4">
         <v>1</v>
@@ -49027,7 +49035,7 @@
         <v>1613</v>
       </c>
       <c r="I670" s="10" t="s">
-        <v>2164</v>
+        <v>2159</v>
       </c>
       <c r="J670" s="4">
         <v>1</v>
@@ -49126,7 +49134,7 @@
         <v>1493</v>
       </c>
       <c r="I673" s="10" t="s">
-        <v>2066</v>
+        <v>2061</v>
       </c>
       <c r="J673" s="4">
         <v>1</v>
@@ -49720,7 +49728,7 @@
         <v>1597</v>
       </c>
       <c r="I691" s="10" t="s">
-        <v>2166</v>
+        <v>2161</v>
       </c>
       <c r="J691" s="4">
         <v>1</v>
@@ -50050,7 +50058,7 @@
         <v>1345</v>
       </c>
       <c r="I701" s="10" t="s">
-        <v>2135</v>
+        <v>2130</v>
       </c>
       <c r="J701" s="4">
         <v>1</v>
@@ -50083,7 +50091,7 @@
         <v>714</v>
       </c>
       <c r="I702" s="10" t="s">
-        <v>2128</v>
+        <v>2123</v>
       </c>
       <c r="J702" s="4">
         <v>1</v>
@@ -50611,7 +50619,7 @@
         <v>714</v>
       </c>
       <c r="I718" s="10" t="s">
-        <v>2129</v>
+        <v>2124</v>
       </c>
       <c r="J718" s="4">
         <v>1</v>
@@ -50644,7 +50652,7 @@
         <v>1579</v>
       </c>
       <c r="I719" s="10" t="s">
-        <v>2141</v>
+        <v>2136</v>
       </c>
       <c r="J719" s="4">
         <v>1</v>
@@ -51040,7 +51048,7 @@
         <v>1466</v>
       </c>
       <c r="I731" s="10" t="s">
-        <v>2094</v>
+        <v>2089</v>
       </c>
       <c r="J731" s="4">
         <v>1</v>
@@ -51501,8 +51509,8 @@
       <c r="H745" s="13" t="s">
         <v>1357</v>
       </c>
-      <c r="I745" s="10" t="s">
-        <v>2055</v>
+      <c r="I745" s="26" t="s">
+        <v>2174</v>
       </c>
       <c r="J745" s="4">
         <v>1</v>
@@ -51568,7 +51576,7 @@
         <v>1416</v>
       </c>
       <c r="I747" s="10" t="s">
-        <v>2115</v>
+        <v>2110</v>
       </c>
       <c r="J747" s="4">
         <v>1</v>
@@ -51832,7 +51840,7 @@
         <v>1358</v>
       </c>
       <c r="I755" s="10" t="s">
-        <v>2092</v>
+        <v>2087</v>
       </c>
       <c r="J755" s="18">
         <v>0</v>
@@ -52096,7 +52104,7 @@
         <v>1358</v>
       </c>
       <c r="I763" s="10" t="s">
-        <v>2093</v>
+        <v>2088</v>
       </c>
       <c r="J763" s="18">
         <v>0</v>
@@ -52228,7 +52236,7 @@
         <v>1350</v>
       </c>
       <c r="I767" s="10" t="s">
-        <v>2152</v>
+        <v>2147</v>
       </c>
       <c r="J767" s="4">
         <v>1</v>
@@ -52261,7 +52269,7 @@
         <v>1426</v>
       </c>
       <c r="I768" s="10" t="s">
-        <v>2173</v>
+        <v>2168</v>
       </c>
       <c r="J768" s="4">
         <v>1</v>
@@ -52393,7 +52401,7 @@
         <v>714</v>
       </c>
       <c r="I772" s="10" t="s">
-        <v>2130</v>
+        <v>2125</v>
       </c>
       <c r="J772" s="4">
         <v>1</v>
@@ -52426,7 +52434,7 @@
         <v>1426</v>
       </c>
       <c r="I773" s="10" t="s">
-        <v>2174</v>
+        <v>2169</v>
       </c>
       <c r="J773" s="4">
         <v>1</v>
@@ -52888,7 +52896,7 @@
         <v>1535</v>
       </c>
       <c r="I787" s="10" t="s">
-        <v>2136</v>
+        <v>2131</v>
       </c>
       <c r="J787" s="4">
         <v>1</v>
@@ -53548,7 +53556,7 @@
         <v>1493</v>
       </c>
       <c r="I807" s="10" t="s">
-        <v>2067</v>
+        <v>2062</v>
       </c>
       <c r="J807" s="4">
         <v>1</v>
@@ -53939,10 +53947,10 @@
       <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="90.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="90.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2">
@@ -58932,9 +58940,9 @@
       <selection activeCell="F30" sqref="F30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.375" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -59797,10 +59805,10 @@
       <selection activeCell="A67" sqref="A67"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="31" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:2">
@@ -59990,9 +59998,9 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="30.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="37.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="61" bestFit="1" customWidth="1"/>
   </cols>
@@ -61586,9 +61594,9 @@
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22.625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="61" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -62243,17 +62251,17 @@
       <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="4"/>
-    <col min="3" max="3" width="30.83203125" style="4" customWidth="1"/>
-    <col min="4" max="8" width="24.83203125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="24.83203125" style="8" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="12" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" style="1"/>
-    <col min="12" max="12" width="10.83203125" style="4"/>
-    <col min="13" max="13" width="20.6640625" style="4" customWidth="1"/>
-    <col min="14" max="16384" width="10.83203125" style="4"/>
+    <col min="1" max="2" width="10.875" style="4"/>
+    <col min="3" max="3" width="30.875" style="4" customWidth="1"/>
+    <col min="4" max="8" width="24.875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="24.875" style="8" customWidth="1"/>
+    <col min="10" max="10" width="11.625" style="12" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.875" style="1"/>
+    <col min="12" max="12" width="10.875" style="4"/>
+    <col min="13" max="13" width="20.625" style="4" customWidth="1"/>
+    <col min="14" max="16384" width="10.875" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="15">

</xml_diff>